<commit_message>
Added support up to 96 wells
</commit_message>
<xml_diff>
--- a/Input/PlateDesignTemplate.xlsx
+++ b/Input/PlateDesignTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\soliscom.uu.nl\Users\Weijg001\My Documents\CodeSpace\ShinyApplications\PlateDesigner\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tweij\Documents\CodeSpace\ShinyApplications\PlateDesignerApp\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71C82FA-2857-4226-B31B-F2DEBE285EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D3B0B6-4AA7-4B16-839F-81F4A808D5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{950F08EF-07BB-4A10-AF0D-0DD602868AD5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="13" xr2:uid="{950F08EF-07BB-4A10-AF0D-0DD602868AD5}"/>
   </bookViews>
   <sheets>
     <sheet name="6well" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="143">
   <si>
     <t>Well</t>
   </si>
@@ -244,6 +244,240 @@
   </si>
   <si>
     <t>LNP6</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>LNP7</t>
+  </si>
+  <si>
+    <t>LNP8</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>LNP9</t>
+  </si>
+  <si>
+    <t>LNP10</t>
+  </si>
+  <si>
+    <t>LNP11</t>
+  </si>
+  <si>
+    <t>LNP12</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>A9</t>
+  </si>
+  <si>
+    <t>B9</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>B10</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>H12</t>
   </si>
 </sst>
 </file>
@@ -281,7 +515,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -304,15 +538,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,9 +702,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +742,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +848,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +990,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,106 +1001,98 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="11">
         <v>10</v>
       </c>
     </row>
@@ -741,12 +1104,477 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9080EC33-19AE-434A-BCD7-951440FEE1C5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>'96well'!B2&amp;"; "&amp;'96well'!C2</f>
+        <v>LNP1; 1</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>'96well'!B10&amp;"; "&amp;'96well'!C10</f>
+        <v>LNP2; 1</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>'96well'!B18&amp;"; "&amp;'96well'!C18</f>
+        <v>LNP3; 1</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>'96well'!B26&amp;"; "&amp;'96well'!C26</f>
+        <v>LNP4; 1</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>'96well'!B34&amp;"; "&amp;'96well'!C34</f>
+        <v>LNP5; 1</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>'96well'!B42&amp;"; "&amp;'96well'!C42</f>
+        <v>LNP6; 1</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>'96well'!B50&amp;"; "&amp;'96well'!C50</f>
+        <v>LNP7; 1</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>'96well'!B58&amp;"; "&amp;'96well'!C58</f>
+        <v>LNP8; 1</v>
+      </c>
+      <c r="J2" s="2" t="str">
+        <f>'96well'!B66&amp;"; "&amp;'96well'!C66</f>
+        <v>LNP9; 1</v>
+      </c>
+      <c r="K2" s="2" t="str">
+        <f>'96well'!B74&amp;"; "&amp;'96well'!C74</f>
+        <v>LNP10; 1</v>
+      </c>
+      <c r="L2" s="2" t="str">
+        <f>'96well'!B82&amp;"; "&amp;'96well'!C82</f>
+        <v>LNP11; 1</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f>'96well'!B90&amp;"; "&amp;'96well'!C90</f>
+        <v>LNP12; 1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>'96well'!B3&amp;"; "&amp;'96well'!C3</f>
+        <v>LNP1; 10</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>'96well'!B11&amp;"; "&amp;'96well'!C11</f>
+        <v>LNP2; 10</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>'96well'!B19&amp;"; "&amp;'96well'!C19</f>
+        <v>LNP3; 10</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>'96well'!B27&amp;"; "&amp;'96well'!C27</f>
+        <v>LNP4; 10</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>'96well'!B35&amp;"; "&amp;'96well'!C35</f>
+        <v>LNP5; 10</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>'96well'!B43&amp;"; "&amp;'96well'!C43</f>
+        <v>LNP6; 10</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>'96well'!B51&amp;"; "&amp;'96well'!C51</f>
+        <v>LNP7; 10</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f>'96well'!B59&amp;"; "&amp;'96well'!C59</f>
+        <v>LNP8; 10</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f>'96well'!B67&amp;"; "&amp;'96well'!C67</f>
+        <v>LNP9; 10</v>
+      </c>
+      <c r="K3" s="2" t="str">
+        <f>'96well'!B75&amp;"; "&amp;'96well'!C75</f>
+        <v>LNP10; 10</v>
+      </c>
+      <c r="L3" s="2" t="str">
+        <f>'96well'!B83&amp;"; "&amp;'96well'!C83</f>
+        <v>LNP11; 10</v>
+      </c>
+      <c r="M3" s="2" t="str">
+        <f>'96well'!B91&amp;"; "&amp;'96well'!C91</f>
+        <v>LNP12; 10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>'96well'!B4&amp;"; "&amp;'96well'!C4</f>
+        <v>LNP1; 100</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>'96well'!B12&amp;"; "&amp;'96well'!C12</f>
+        <v>LNP2; 100</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>'96well'!B20&amp;"; "&amp;'96well'!C20</f>
+        <v>LNP3; 100</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f>'96well'!B28&amp;"; "&amp;'96well'!C28</f>
+        <v>LNP4; 100</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f>'96well'!B36&amp;"; "&amp;'96well'!C36</f>
+        <v>LNP5; 100</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f>'96well'!B44&amp;"; "&amp;'96well'!C44</f>
+        <v>LNP6; 100</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>'96well'!B52&amp;"; "&amp;'96well'!C52</f>
+        <v>LNP7; 100</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>'96well'!B60&amp;"; "&amp;'96well'!C60</f>
+        <v>LNP8; 100</v>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f>'96well'!B68&amp;"; "&amp;'96well'!C68</f>
+        <v>LNP9; 100</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>'96well'!B76&amp;"; "&amp;'96well'!C76</f>
+        <v>LNP10; 100</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>'96well'!B84&amp;"; "&amp;'96well'!C84</f>
+        <v>LNP11; 100</v>
+      </c>
+      <c r="M4" s="2" t="str">
+        <f>'96well'!B92&amp;"; "&amp;'96well'!C92</f>
+        <v>LNP12; 100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>'96well'!B5&amp;"; "&amp;'96well'!C5</f>
+        <v>LNP1; 200</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>'96well'!B13&amp;"; "&amp;'96well'!C13</f>
+        <v>LNP2; 200</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>'96well'!B21&amp;"; "&amp;'96well'!C21</f>
+        <v>LNP3; 200</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>'96well'!B29&amp;"; "&amp;'96well'!C29</f>
+        <v>LNP4; 200</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f>'96well'!B37&amp;"; "&amp;'96well'!C37</f>
+        <v>LNP5; 200</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f>'96well'!B45&amp;"; "&amp;'96well'!C45</f>
+        <v>LNP6; 200</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f>'96well'!B53&amp;"; "&amp;'96well'!C53</f>
+        <v>LNP7; 200</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f>'96well'!B61&amp;"; "&amp;'96well'!C61</f>
+        <v>LNP8; 200</v>
+      </c>
+      <c r="J5" s="2" t="str">
+        <f>'96well'!B69&amp;"; "&amp;'96well'!C69</f>
+        <v>LNP9; 200</v>
+      </c>
+      <c r="K5" s="2" t="str">
+        <f>'96well'!B77&amp;"; "&amp;'96well'!C77</f>
+        <v>LNP10; 200</v>
+      </c>
+      <c r="L5" s="2" t="str">
+        <f>'96well'!B85&amp;"; "&amp;'96well'!C85</f>
+        <v>LNP11; 200</v>
+      </c>
+      <c r="M5" s="2" t="str">
+        <f>'96well'!B93&amp;"; "&amp;'96well'!C93</f>
+        <v>LNP12; 200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>'96well'!B6&amp;"; "&amp;'96well'!C6</f>
+        <v>LNP1; 400</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>'96well'!B14&amp;"; "&amp;'96well'!C14</f>
+        <v>LNP2; 400</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>'96well'!B22&amp;"; "&amp;'96well'!C22</f>
+        <v>LNP3; 400</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>'96well'!B30&amp;"; "&amp;'96well'!C30</f>
+        <v>LNP4; 400</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f>'96well'!B38&amp;"; "&amp;'96well'!C38</f>
+        <v>LNP5; 400</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f>'96well'!B46&amp;"; "&amp;'96well'!C46</f>
+        <v>LNP6; 400</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f>'96well'!B54&amp;"; "&amp;'96well'!C54</f>
+        <v>LNP7; 400</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>'96well'!B62&amp;"; "&amp;'96well'!C62</f>
+        <v>LNP8; 400</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>'96well'!B70&amp;"; "&amp;'96well'!C70</f>
+        <v>LNP9; 400</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f>'96well'!B78&amp;"; "&amp;'96well'!C78</f>
+        <v>LNP10; 400</v>
+      </c>
+      <c r="L6" s="2" t="str">
+        <f>'96well'!B86&amp;"; "&amp;'96well'!C86</f>
+        <v>LNP11; 400</v>
+      </c>
+      <c r="M6" s="2" t="str">
+        <f>'96well'!B94&amp;"; "&amp;'96well'!C94</f>
+        <v>LNP12; 400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>'96well'!B7&amp;"; "&amp;'96well'!C7</f>
+        <v>LNP1; 600</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>'96well'!B15&amp;"; "&amp;'96well'!C15</f>
+        <v>LNP2; 600</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>'96well'!B23&amp;"; "&amp;'96well'!C23</f>
+        <v>LNP3; 600</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>'96well'!B31&amp;"; "&amp;'96well'!C31</f>
+        <v>LNP4; 600</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f>'96well'!B39&amp;"; "&amp;'96well'!C39</f>
+        <v>LNP5; 600</v>
+      </c>
+      <c r="G7" s="2" t="str">
+        <f>'96well'!B47&amp;"; "&amp;'96well'!C47</f>
+        <v>LNP6; 600</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>'96well'!B55&amp;"; "&amp;'96well'!C55</f>
+        <v>LNP7; 600</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f>'96well'!B63&amp;"; "&amp;'96well'!C63</f>
+        <v>LNP8; 600</v>
+      </c>
+      <c r="J7" s="2" t="str">
+        <f>'96well'!B71&amp;"; "&amp;'96well'!C71</f>
+        <v>LNP9; 600</v>
+      </c>
+      <c r="K7" s="2" t="str">
+        <f>'96well'!B79&amp;"; "&amp;'96well'!C79</f>
+        <v>LNP10; 600</v>
+      </c>
+      <c r="L7" s="2" t="str">
+        <f>'96well'!B87&amp;"; "&amp;'96well'!C87</f>
+        <v>LNP11; 600</v>
+      </c>
+      <c r="M7" s="2" t="str">
+        <f>'96well'!B95&amp;"; "&amp;'96well'!C95</f>
+        <v>LNP12; 600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="str">
+        <f>'96well'!B8&amp;"; "&amp;'96well'!C8</f>
+        <v>LNP1; 800</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>'96well'!B16&amp;"; "&amp;'96well'!C16</f>
+        <v>LNP2; 800</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f>'96well'!B24&amp;"; "&amp;'96well'!C24</f>
+        <v>LNP3; 800</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f>'96well'!B32&amp;"; "&amp;'96well'!C32</f>
+        <v>LNP4; 800</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f>'96well'!B40&amp;"; "&amp;'96well'!C40</f>
+        <v>LNP5; 800</v>
+      </c>
+      <c r="G8" s="2" t="str">
+        <f>'96well'!B48&amp;"; "&amp;'96well'!C48</f>
+        <v>LNP6; 800</v>
+      </c>
+      <c r="H8" s="2" t="str">
+        <f>'96well'!B56&amp;"; "&amp;'96well'!C56</f>
+        <v>LNP7; 800</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f>'96well'!B64&amp;"; "&amp;'96well'!C64</f>
+        <v>LNP8; 800</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f>'96well'!B72&amp;"; "&amp;'96well'!C72</f>
+        <v>LNP9; 800</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f>'96well'!B80&amp;"; "&amp;'96well'!C80</f>
+        <v>LNP10; 800</v>
+      </c>
+      <c r="L8" s="2" t="str">
+        <f>'96well'!B88&amp;"; "&amp;'96well'!C88</f>
+        <v>LNP11; 800</v>
+      </c>
+      <c r="M8" s="2" t="str">
+        <f>'96well'!B96&amp;"; "&amp;'96well'!C96</f>
+        <v>LNP12; 800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="str">
+        <f>'96well'!B9&amp;"; "&amp;'96well'!C9</f>
+        <v>LNP1; 1000</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f>'96well'!B17&amp;"; "&amp;'96well'!C17</f>
+        <v>LNP2; 1000</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>'96well'!B25&amp;"; "&amp;'96well'!C25</f>
+        <v>LNP3; 1000</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f>'96well'!B33&amp;"; "&amp;'96well'!C33</f>
+        <v>LNP4; 1000</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f>'96well'!B41&amp;"; "&amp;'96well'!C41</f>
+        <v>LNP5; 1000</v>
+      </c>
+      <c r="G9" s="2" t="str">
+        <f>'96well'!B49&amp;"; "&amp;'96well'!C49</f>
+        <v>LNP6; 1000</v>
+      </c>
+      <c r="H9" s="2" t="str">
+        <f>'96well'!B57&amp;"; "&amp;'96well'!C57</f>
+        <v>LNP7; 1000</v>
+      </c>
+      <c r="I9" s="2" t="str">
+        <f>'96well'!B65&amp;"; "&amp;'96well'!C65</f>
+        <v>LNP8; 1000</v>
+      </c>
+      <c r="J9" s="2" t="str">
+        <f>'96well'!B73&amp;"; "&amp;'96well'!C73</f>
+        <v>LNP9; 1000</v>
+      </c>
+      <c r="K9" s="2" t="str">
+        <f>'96well'!B81&amp;"; "&amp;'96well'!C81</f>
+        <v>LNP10; 1000</v>
+      </c>
+      <c r="L9" s="2" t="str">
+        <f>'96well'!B89&amp;"; "&amp;'96well'!C89</f>
+        <v>LNP11; 1000</v>
+      </c>
+      <c r="M9" s="2" t="str">
+        <f>'96well'!B97&amp;"; "&amp;'96well'!C97</f>
+        <v>LNP12; 1000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -757,7 +1585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -769,7 +1597,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -781,7 +1609,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -791,13 +1619,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4B4792-059E-4367-A89C-466DD357EB94}">
   <dimension ref="A1:AW33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
@@ -943,7 +1771,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -996,7 +1824,7 @@
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1877,7 @@
       <c r="AV3" s="2"/>
       <c r="AW3" s="2"/>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1102,7 +1930,7 @@
       <c r="AV4" s="2"/>
       <c r="AW4" s="2"/>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +1983,7 @@
       <c r="AV5" s="2"/>
       <c r="AW5" s="2"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1208,7 +2036,7 @@
       <c r="AV6" s="2"/>
       <c r="AW6" s="2"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1261,7 +2089,7 @@
       <c r="AV7" s="2"/>
       <c r="AW7" s="2"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1314,7 +2142,7 @@
       <c r="AV8" s="2"/>
       <c r="AW8" s="2"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1367,7 +2195,7 @@
       <c r="AV9" s="2"/>
       <c r="AW9" s="2"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1420,7 +2248,7 @@
       <c r="AV10" s="2"/>
       <c r="AW10" s="2"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1473,7 +2301,7 @@
       <c r="AV11" s="2"/>
       <c r="AW11" s="2"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1526,7 +2354,7 @@
       <c r="AV12" s="2"/>
       <c r="AW12" s="2"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1579,7 +2407,7 @@
       <c r="AV13" s="2"/>
       <c r="AW13" s="2"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1632,7 +2460,7 @@
       <c r="AV14" s="2"/>
       <c r="AW14" s="2"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1685,7 +2513,7 @@
       <c r="AV15" s="2"/>
       <c r="AW15" s="2"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1738,7 +2566,7 @@
       <c r="AV16" s="2"/>
       <c r="AW16" s="2"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1791,7 +2619,7 @@
       <c r="AV17" s="2"/>
       <c r="AW17" s="2"/>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1844,7 +2672,7 @@
       <c r="AV18" s="2"/>
       <c r="AW18" s="2"/>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1897,7 +2725,7 @@
       <c r="AV19" s="2"/>
       <c r="AW19" s="2"/>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1950,7 +2778,7 @@
       <c r="AV20" s="2"/>
       <c r="AW20" s="2"/>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -2003,7 +2831,7 @@
       <c r="AV21" s="2"/>
       <c r="AW21" s="2"/>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -2056,7 +2884,7 @@
       <c r="AV22" s="2"/>
       <c r="AW22" s="2"/>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -2109,7 +2937,7 @@
       <c r="AV23" s="2"/>
       <c r="AW23" s="2"/>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -2162,7 +2990,7 @@
       <c r="AV24" s="2"/>
       <c r="AW24" s="2"/>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -2215,7 +3043,7 @@
       <c r="AV25" s="2"/>
       <c r="AW25" s="2"/>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2268,7 +3096,7 @@
       <c r="AV26" s="2"/>
       <c r="AW26" s="2"/>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -2321,7 +3149,7 @@
       <c r="AV27" s="2"/>
       <c r="AW27" s="2"/>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2374,7 +3202,7 @@
       <c r="AV28" s="2"/>
       <c r="AW28" s="2"/>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2427,7 +3255,7 @@
       <c r="AV29" s="2"/>
       <c r="AW29" s="2"/>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2480,7 +3308,7 @@
       <c r="AV30" s="2"/>
       <c r="AW30" s="2"/>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +3361,7 @@
       <c r="AV31" s="2"/>
       <c r="AW31" s="2"/>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2586,7 +3414,7 @@
       <c r="AV32" s="2"/>
       <c r="AW32" s="2"/>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -2652,22 +3480,21 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="6" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="6" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B1">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1">
         <v>2</v>
       </c>
       <c r="D1">
@@ -2677,8 +3504,8 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="str">
@@ -2694,7 +3521,7 @@
         <v>LNP3; 1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2718,167 +3545,158 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1082C8EF-D562-4654-9520-2409F48CF315}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="A1:C13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="11">
         <v>100</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="11">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="11">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="11">
         <v>100</v>
       </c>
     </row>
@@ -2896,12 +3714,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
@@ -2918,7 +3736,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2939,7 +3757,7 @@
         <v>LNP4; 1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2960,7 +3778,7 @@
         <v>LNP4; 10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2988,405 +3806,291 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB25A04-FF01-4E4A-A76D-1F2392716AB0}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>10</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>100</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="11">
         <v>1000</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>10</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>100</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="11">
         <v>1000</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
         <v>10</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="8">
         <v>100</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="11">
         <v>1000</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>1</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="8">
         <v>10</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="8">
         <v>100</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="11">
         <v>1000</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>1</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="8">
         <v>10</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="11">
         <v>1000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="11">
         <v>1000</v>
       </c>
     </row>
@@ -3400,13 +4104,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41B9D619-C28E-4B3F-A596-3C22CF59F121}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>1</v>
       </c>
@@ -3426,7 +4130,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -3455,7 +4159,7 @@
         <v>LNP6; 1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3484,7 +4188,7 @@
         <v>LNP6; 10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3513,7 +4217,7 @@
         <v>LNP6; 100</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3549,36 +4253,1907 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A67CC51-F918-4126-8D26-01D27FB10C75}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{090C15FD-E2DF-46DB-8EEF-F80D097FFC17}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="A1:J9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="str">
+        <f>'48well'!B2&amp;"; "&amp;'48well'!C2</f>
+        <v>LNP1; 1</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>'48well'!B8&amp;"; "&amp;'48well'!C8</f>
+        <v>LNP2; 1</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f>'48well'!B14&amp;"; "&amp;'48well'!C14</f>
+        <v>LNP3; 1</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>'48well'!B20&amp;"; "&amp;'48well'!C20</f>
+        <v>LNP4; 1</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f>'48well'!B26&amp;"; "&amp;'48well'!C26</f>
+        <v>LNP5; 1</v>
+      </c>
+      <c r="G2" s="2" t="str">
+        <f>'48well'!B32&amp;"; "&amp;'48well'!C32</f>
+        <v>LNP6; 1</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f>'48well'!B38&amp;"; "&amp;'48well'!C38</f>
+        <v>LNP7; 1</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>'48well'!B44&amp;"; "&amp;'48well'!C44</f>
+        <v>LNP8; 1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>'48well'!B3&amp;"; "&amp;'48well'!C3</f>
+        <v>LNP1; 10</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>'48well'!B9&amp;"; "&amp;'48well'!C9</f>
+        <v>LNP2; 10</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>'48well'!B15&amp;"; "&amp;'48well'!C15</f>
+        <v>LNP3; 10</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>'48well'!B21&amp;"; "&amp;'48well'!C21</f>
+        <v>LNP4; 10</v>
+      </c>
+      <c r="F3" s="2" t="str">
+        <f>'48well'!B27&amp;"; "&amp;'48well'!C27</f>
+        <v>LNP5; 10</v>
+      </c>
+      <c r="G3" s="2" t="str">
+        <f>'48well'!B33&amp;"; "&amp;'48well'!C33</f>
+        <v>LNP6; 10</v>
+      </c>
+      <c r="H3" s="2" t="str">
+        <f>'48well'!B39&amp;"; "&amp;'48well'!C39</f>
+        <v>LNP7; 10</v>
+      </c>
+      <c r="I3" s="2" t="str">
+        <f>'48well'!B45&amp;"; "&amp;'48well'!C45</f>
+        <v>LNP8; 10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="str">
+        <f>'48well'!B4&amp;"; "&amp;'48well'!C4</f>
+        <v>LNP1; 100</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>'48well'!B10&amp;"; "&amp;'48well'!C10</f>
+        <v>LNP2; 100</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>'48well'!B16&amp;"; "&amp;'48well'!C16</f>
+        <v>LNP3; 100</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f>'48well'!B22&amp;"; "&amp;'48well'!C22</f>
+        <v>LNP4; 100</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f>'48well'!B28&amp;"; "&amp;'48well'!C28</f>
+        <v>LNP5; 100</v>
+      </c>
+      <c r="G4" s="2" t="str">
+        <f>'48well'!B34&amp;"; "&amp;'48well'!C34</f>
+        <v>LNP6; 100</v>
+      </c>
+      <c r="H4" s="2" t="str">
+        <f>'48well'!B40&amp;"; "&amp;'48well'!C40</f>
+        <v>LNP7; 100</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>'48well'!B46&amp;"; "&amp;'48well'!C46</f>
+        <v>LNP8; 100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>'48well'!B5&amp;"; "&amp;'48well'!C5</f>
+        <v>LNP1; 200</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>'48well'!B11&amp;"; "&amp;'48well'!C11</f>
+        <v>LNP2; 200</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>'48well'!B17&amp;"; "&amp;'48well'!C17</f>
+        <v>LNP3; 200</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>'48well'!B23&amp;"; "&amp;'48well'!C23</f>
+        <v>LNP4; 200</v>
+      </c>
+      <c r="F5" s="2" t="str">
+        <f>'48well'!B29&amp;"; "&amp;'48well'!C29</f>
+        <v>LNP5; 200</v>
+      </c>
+      <c r="G5" s="2" t="str">
+        <f>'48well'!B35&amp;"; "&amp;'48well'!C35</f>
+        <v>LNP6; 200</v>
+      </c>
+      <c r="H5" s="2" t="str">
+        <f>'48well'!B41&amp;"; "&amp;'48well'!C41</f>
+        <v>LNP7; 200</v>
+      </c>
+      <c r="I5" s="2" t="str">
+        <f>'48well'!B47&amp;"; "&amp;'48well'!C47</f>
+        <v>LNP8; 200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="str">
+        <f>'48well'!B6&amp;"; "&amp;'48well'!C6</f>
+        <v>LNP1; 400</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>'48well'!B12&amp;"; "&amp;'48well'!C12</f>
+        <v>LNP2; 400</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f>'48well'!B18&amp;"; "&amp;'48well'!C18</f>
+        <v>LNP3; 400</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>'48well'!B24&amp;"; "&amp;'48well'!C24</f>
+        <v>LNP4; 400</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f>'48well'!B30&amp;"; "&amp;'48well'!C30</f>
+        <v>LNP5; 400</v>
+      </c>
+      <c r="G6" s="2" t="str">
+        <f>'48well'!B36&amp;"; "&amp;'48well'!C36</f>
+        <v>LNP6; 400</v>
+      </c>
+      <c r="H6" s="2" t="str">
+        <f>'48well'!B42&amp;"; "&amp;'48well'!C42</f>
+        <v>LNP7; 400</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>'48well'!B48&amp;"; "&amp;'48well'!C48</f>
+        <v>LNP8; 400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="str">
+        <f>'48well'!B7&amp;"; "&amp;'48well'!C7</f>
+        <v>LNP1; 1000</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>'48well'!B13&amp;"; "&amp;'48well'!C13</f>
+        <v>LNP2; 1000</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>'48well'!B19&amp;"; "&amp;'48well'!C19</f>
+        <v>LNP3; 1000</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>'48well'!B25&amp;"; "&amp;'48well'!C25</f>
+        <v>LNP4; 1000</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f>'48well'!B31&amp;"; "&amp;'48well'!C31</f>
+        <v>LNP5; 1000</v>
+      </c>
+      <c r="G7" s="2" t="str">
+        <f>'48well'!B37&amp;"; "&amp;'48well'!C37</f>
+        <v>LNP6; 1000</v>
+      </c>
+      <c r="H7" s="2" t="str">
+        <f>'48well'!B43&amp;"; "&amp;'48well'!C43</f>
+        <v>LNP7; 1000</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <f>'48well'!B49&amp;"; "&amp;'48well'!C49</f>
+        <v>LNP8; 1000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0892F86D-3DB5-41E0-9884-B5D565FB53F7}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C44" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C52" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C61" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C62" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C64" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C65" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C66" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C70" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C71" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C72" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C73" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C74" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C76" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C77" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C79" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C80" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C82" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C84" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C89" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C90" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C91" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C92" s="8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C94" s="8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C95" s="8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C96" s="8">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C97" s="11">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>